<commit_message>
feat: compiling to manylinux
</commit_message>
<xml_diff>
--- a/text.xlsx
+++ b/text.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -486,7 +486,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -536,7 +536,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -636,7 +636,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -761,7 +761,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -836,7 +836,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -861,7 +861,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ADerkachev</t>
+          <t>PRIVET_FROM_PARSER!</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">

</xml_diff>